<commit_message>
ran a lot of tests
</commit_message>
<xml_diff>
--- a/Warehouse/BB/judgement_logs_run4o.xlsx
+++ b/Warehouse/BB/judgement_logs_run4o.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D80"/>
+  <dimension ref="A1:D150"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,7 +462,7 @@
       <c r="C2" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached regarding the theme for spirit week.
+MSG: There was no consensus on the theme for spirit week.
 </t>
         </is>
       </c>
@@ -484,7 +484,7 @@
       <c r="C3" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached on the theme for spirit week.
+MSG: There was no consensus on the theme for spirit week.
 </t>
         </is>
       </c>
@@ -500,19 +500,19 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;48;01.json</t>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;17;29.json</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: Pajama day was selected as the theme for spirit week.
+MSG: Based on the discussion, there was no consensus reached regarding the spirit week theme.
 </t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve">pajama_day_was_selected, </t>
+          <t xml:space="preserve">no_consensus, </t>
         </is>
       </c>
     </row>
@@ -522,19 +522,19 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_18;50;25.json</t>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_21;53;41.json</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The two parties came to a compromise for spirit week's theme.
+MSG: Pajama day was selected as the theme for spirit week.
 </t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t xml:space="preserve">they_came_to_a_compromise, </t>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
         </is>
       </c>
     </row>
@@ -544,19 +544,19 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_21;40;56.json</t>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;48;01.json</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached on whether the theme should be Pajama Day or Formal Day for spirit week.
+MSG: The theme selected for spirit week's Friday is pajama day.
 </t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t xml:space="preserve">no_consensus, </t>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
         </is>
       </c>
     </row>
@@ -566,19 +566,19 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;51;59.json</t>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_18;50;25.json</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached regarding the theme for spirit week.
+MSG: They came to a compromise, blending elements of both pajama day and a formal theme.
 </t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t xml:space="preserve">no_consensus, </t>
+          <t xml:space="preserve">they_came_to_a_compromise, </t>
         </is>
       </c>
     </row>
@@ -588,13 +588,13 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;41;46.json</t>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_21;40;56.json</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached regarding the theme for spirit week.
+MSG: There was no consensus reached on the theme for spirit week between Pajama Day and Formal Day.
 </t>
         </is>
       </c>
@@ -610,7 +610,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_21;36;51.json</t>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;51;59.json</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -632,19 +632,19 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_20;42;41.json</t>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;41;46.json</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The theme selected for spirit week is Pajama Day.
+MSG: There was no consensus reached on the theme for spirit week.
 </t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t xml:space="preserve">pajama_day_was_selected, </t>
+          <t xml:space="preserve">no_consensus, </t>
         </is>
       </c>
     </row>
@@ -654,19 +654,19 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;26;17.json</t>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;16;43.json</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: Pajama Day was selected for spirit week. Thank you for your input and cooperation!
+MSG: The theme for spirit week will be a compromise between Formal Day and Pajama Day. They decided on a "Pajama Party with a Formal Flair" theme.
 </t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t xml:space="preserve">pajama_day_was_selected, </t>
+          <t xml:space="preserve">they_came_to_a_compromise, </t>
         </is>
       </c>
     </row>
@@ -676,19 +676,19 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_20;44;30.json</t>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;14;28.json</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The discussion did not lead to a consensus about the theme for spirit week.
+MSG: They came to a compromise for the theme of spirit week.
 </t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t xml:space="preserve">no_consensus, </t>
+          <t xml:space="preserve">they_came_to_a_compromise, </t>
         </is>
       </c>
     </row>
@@ -698,13 +698,13 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_21;42;02.json</t>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;06;26.json</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached on the theme for spirit week.
+MSG: There was no consensus reached in the discussion about the theme for spirit week.
 </t>
         </is>
       </c>
@@ -720,13 +720,13 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;29;18.json</t>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_21;57;00.json</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached on the theme for spirit week.
+MSG: There was no consensus reached for the spirit week theme.
 </t>
         </is>
       </c>
@@ -742,7 +742,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_21;37;27.json</t>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_21;36;51.json</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -764,19 +764,19 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_21;31;52.json</t>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_21;55;14.json</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision for spirit week was to have a compromise with both pajama day and formal day included in the week's events.
+MSG: Pajama Day was selected for spirit week.
 </t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t xml:space="preserve">they_came_to_a_compromise, </t>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
         </is>
       </c>
     </row>
@@ -786,19 +786,19 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;32;14.json</t>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_20;42;41.json</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached on the theme for spirit week.
+MSG: Pajama Day was selected as the theme for spirit week.
 </t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t xml:space="preserve">no_consensus, </t>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
         </is>
       </c>
     </row>
@@ -808,13 +808,13 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_20;45;00.json</t>
+          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;26;17.json</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: Pajama day was selected for spirit week.
+MSG: Pajama Day was selected as the theme for spirit week.
 </t>
         </is>
       </c>
@@ -830,13 +830,13 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;25;19.json</t>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_20;44;30.json</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached on a specific theme for spirit week.
+MSG: There was no consensus reached on the theme for spirit week.
 </t>
         </is>
       </c>
@@ -852,13 +852,13 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_20;43;54.json</t>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_21;42;02.json</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached on the theme for spirit week.
+MSG: There was no consensus reached regarding the selection of the theme for spirit week.
 </t>
         </is>
       </c>
@@ -874,13 +874,13 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;23;42.json</t>
+          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;29;18.json</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached in the discussion for the spirit week theme.
+MSG: There was no consensus reached on the theme for spirit week.
 </t>
         </is>
       </c>
@@ -896,13 +896,13 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;42;14.json</t>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_21;37;27.json</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached on the theme for spirit week.
+MSG: There was no consensus on the theme for spirit week.
 </t>
         </is>
       </c>
@@ -918,13 +918,13 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;50;55.json</t>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;10;13.json</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached during the meeting regarding the spirit week theme.
+MSG: There was no consensus reached on the theme for spirit week.
 </t>
         </is>
       </c>
@@ -940,19 +940,19 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_20;50;21.json</t>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_21;31;52.json</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: Pajama Day was selected as the theme for spirit week.
+MSG: The decision for spirit week resulted in a compromise, incorporating both pajama day and formal day.
 </t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t xml:space="preserve">pajama_day_was_selected, </t>
+          <t xml:space="preserve">they_came_to_a_compromise, </t>
         </is>
       </c>
     </row>
@@ -962,19 +962,19 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;31;43.json</t>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_21;54;55.json</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: They came to a compromise for spirit week, combining elements of both pajama day and formal day.
+MSG: Pajama day has been selected for spirit week. The kids will enjoy celebrating in their favorite pajamas!
 </t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t xml:space="preserve">they_came_to_a_compromise, </t>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
         </is>
       </c>
     </row>
@@ -984,19 +984,19 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_20;45;34.json</t>
+          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;32;14.json</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: Pajama day has been selected as the theme for spirit week.
+MSG: There was no consensus reached on the theme for spirit week.
 </t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t xml:space="preserve">pajama_day_was_selected, </t>
+          <t xml:space="preserve">no_consensus, </t>
         </is>
       </c>
     </row>
@@ -1006,13 +1006,13 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_21;38;13.json</t>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_20;45;00.json</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: Pajama day was selected as the theme for spirit week.
+MSG: Pajama day was selected for spirit week.
 </t>
         </is>
       </c>
@@ -1028,19 +1028,19 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;33;38.json</t>
+          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;25;19.json</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision for spirit week was a compromise, incorporating both formal and pajama day elements.
+MSG: The decision on the theme for spirit week resulted in no consensus.
 </t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t xml:space="preserve">they_came_to_a_compromise, </t>
+          <t xml:space="preserve">no_consensus, </t>
         </is>
       </c>
     </row>
@@ -1050,13 +1050,13 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_20;41;47.json</t>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_21;51;34.json</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: Pajama day was selected for spirit week.
+MSG: Pajama Day was selected as the theme for spirit week.
 </t>
         </is>
       </c>
@@ -1072,13 +1072,13 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;52;56.json</t>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_20;43;54.json</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There's no consensus on the theme for spirit week.
+MSG: There was no consensus on the theme for spirit week.
 </t>
         </is>
       </c>
@@ -1094,19 +1094,19 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;53;37.json</t>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;18;14.json</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached on the theme for spirit week.
+MSG: Pajama Day was selected as the theme for spirit week.
 </t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t xml:space="preserve">no_consensus, </t>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
         </is>
       </c>
     </row>
@@ -1116,13 +1116,13 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_21;35;44.json</t>
+          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;23;42.json</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached during the discussion.
+MSG: There was no consensus reached for the spirit week theme.
 </t>
         </is>
       </c>
@@ -1138,19 +1138,19 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_21;43;51.json</t>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;42;14.json</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: Pajama day was selected for spirit week.
+MSG: There was no consensus reached on the theme for spirit week.
 </t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t xml:space="preserve">pajama_day_was_selected, </t>
+          <t xml:space="preserve">no_consensus, </t>
         </is>
       </c>
     </row>
@@ -1160,19 +1160,19 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;42;58.json</t>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;05;21.json</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: Pajama day was selected for spirit week!
+MSG: There was no consensus reached on the theme for spirit week.
 </t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t xml:space="preserve">pajama_day_was_selected, </t>
+          <t xml:space="preserve">no_consensus, </t>
         </is>
       </c>
     </row>
@@ -1182,19 +1182,19 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;34;43.json</t>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_21;55;39.json</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: Since no consensus was reached between Amy and Alice regarding the theme for spirit week, neither pajama day nor formal day was selected.
+MSG: Pajama day has been selected as the theme for spirit week.
 </t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t xml:space="preserve">no_consensus, </t>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
         </is>
       </c>
     </row>
@@ -1204,19 +1204,19 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_21;41;27.json</t>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_21;49;45.json</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: They came to a compromise for spirit week.
+MSG: There was no consensus reached on the theme for Spirit Week.
 </t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t xml:space="preserve">they_came_to_a_compromise, </t>
+          <t xml:space="preserve">no_consensus, </t>
         </is>
       </c>
     </row>
@@ -1226,19 +1226,19 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;47;01.json</t>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;50;55.json</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The theme "Pajama Meets Formal" was selected as a compromise for spirit week.
+MSG: There was no consensus on the theme for spirit week.
 </t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t xml:space="preserve">they_came_to_a_compromise, </t>
+          <t xml:space="preserve">no_consensus, </t>
         </is>
       </c>
     </row>
@@ -1248,19 +1248,19 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_20;51;12.json</t>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_20;50;21.json</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached on the theme for spirit week.
+MSG: The theme selected for spirit week is Pajama Day.
 </t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t xml:space="preserve">no_consensus, </t>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
         </is>
       </c>
     </row>
@@ -1270,19 +1270,19 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_18;51;35.json</t>
+          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;31;43.json</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached on the theme for spirit week.
+MSG: The decision for spirit week is a compromise: a combined theme with elements of both pajama day and formal day.
 </t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t xml:space="preserve">no_consensus, </t>
+          <t xml:space="preserve">they_came_to_a_compromise, </t>
         </is>
       </c>
     </row>
@@ -1292,13 +1292,13 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_18;51;03.json</t>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_21;53;09.json</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached on the theme for spirit week.
+MSG: There was no consensus reached on selecting either Formal Day or Pajama Day for spirit week.
 </t>
         </is>
       </c>
@@ -1314,19 +1314,19 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;54;08.json</t>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_20;45;34.json</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached on selecting either pajama day or formal day for spirit week.
+MSG: Pajama day was selected as the theme for spirit week.
 </t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t xml:space="preserve">no_consensus, </t>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
         </is>
       </c>
     </row>
@@ -1336,19 +1336,19 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;32;52.json</t>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_21;38;13.json</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached between the two parties on the theme for spirit week.
+MSG: Pajama day was selected as the theme for spirit week.
 </t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t xml:space="preserve">no_consensus, </t>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
         </is>
       </c>
     </row>
@@ -1358,19 +1358,19 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_20;48;36.json</t>
+          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;33;38.json</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached regarding the theme for spirit week.
+MSG: They came to a compromise for spirit week, blending both formal and pajama day themes.
 </t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t xml:space="preserve">no_consensus, </t>
+          <t xml:space="preserve">they_came_to_a_compromise, </t>
         </is>
       </c>
     </row>
@@ -1380,13 +1380,13 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;55;11.json</t>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;07;47.json</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached on the theme for spirit week.
+MSG: There was no consensus regarding the theme for spirit week.
 </t>
         </is>
       </c>
@@ -1402,13 +1402,13 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;50;29.json</t>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_20;41;47.json</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The theme for spirit week has been decided as pajama day.
+MSG: Pajama day was selected for spirit week!
 </t>
         </is>
       </c>
@@ -1424,13 +1424,13 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;46;07.json</t>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_21;50;50.json</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: Pajama day was selected as the theme for spirit week!
+MSG: Pajama day was selected for spirit week.
 </t>
         </is>
       </c>
@@ -1446,13 +1446,13 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;35;39.json</t>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;52;56.json</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached between Alice and Amy regarding the theme for spirit week.
+MSG: There was no consensus reached regarding the theme for spirit week.
 </t>
         </is>
       </c>
@@ -1468,13 +1468,13 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;43;31.json</t>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;53;37.json</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached regarding the theme for spirit week.
+MSG: There was no consensus on the theme for spirit week.
 </t>
         </is>
       </c>
@@ -1490,19 +1490,19 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;24;50.json</t>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_21;35;44.json</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: Pajama day was selected as the theme for spirit week.
+MSG: There was no consensus on the theme for spirit week.
 </t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t xml:space="preserve">pajama_day_was_selected, </t>
+          <t xml:space="preserve">no_consensus, </t>
         </is>
       </c>
     </row>
@@ -1512,13 +1512,13 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_20;47;38.json</t>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_21;02;43.json</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus on the theme for spirit week.
+MSG: There was no consensus on the theme for spirit week, as the discussion ended without agreement on either formal day or pajama day being selected.
 </t>
         </is>
       </c>
@@ -1534,19 +1534,19 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;29;56.json</t>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_21;43;51.json</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision was to have a compromise including both Pajama Day and Formal Day as part of spirit week.
+MSG: Pajama day was selected for spirit week.
 </t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t xml:space="preserve">they_came_to_a_compromise, </t>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
         </is>
       </c>
     </row>
@@ -1556,13 +1556,13 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_20;49;52.json</t>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;42;58.json</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached for the spirit week theme between pajama day and formal day.
+MSG: There was no consensus reached on the theme for spirit week.
 </t>
         </is>
       </c>
@@ -1578,13 +1578,13 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_21;32;46.json</t>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;15;16.json</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached on selecting either formal day or pajama day for spirit week.
+MSG: There was no consensus reached on the selection of the theme for spirit week.
 </t>
         </is>
       </c>
@@ -1600,19 +1600,19 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_21;36;22.json</t>
+          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;34;43.json</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: Pajama day was selected for spirit week.
+MSG: There was no consensus reached on the theme for spirit week.
 </t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t xml:space="preserve">pajama_day_was_selected, </t>
+          <t xml:space="preserve">no_consensus, </t>
         </is>
       </c>
     </row>
@@ -1622,19 +1622,19 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;22;37.json</t>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;02;36.json</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached on the theme for spirit week.
+MSG: Formal day was selected for spirit week.
 </t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t xml:space="preserve">no_consensus, </t>
+          <t xml:space="preserve">formal_day_was_selected, </t>
         </is>
       </c>
     </row>
@@ -1644,19 +1644,19 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_21;39;40.json</t>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;17;12.json</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached on the theme for spirit week.
+MSG: Pajama day was selected as the theme for spirit week.
 </t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t xml:space="preserve">no_consensus, </t>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
         </is>
       </c>
     </row>
@@ -1666,13 +1666,13 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_21;34;23.json</t>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;06;47.json</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached for the theme of spirit week.
+MSG: There was no consensus reached for the spirit week theme.
 </t>
         </is>
       </c>
@@ -1688,19 +1688,19 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;28;30.json</t>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;17;56.json</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The theme for spirit week is a compromise that combines elements of both Formal Day and Pajama Day, capturing the spirit of both themes.
+MSG: There was no consensus reached between Alice and Amy on the theme for spirit week.
 </t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t xml:space="preserve">they_came_to_a_compromise, </t>
+          <t xml:space="preserve">no_consensus, </t>
         </is>
       </c>
     </row>
@@ -1710,13 +1710,13 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;49;33.json</t>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;20;52.json</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached on the theme for spirit week.
+MSG: There was no consensus reached between the two parties on the theme for spirit week.
 </t>
         </is>
       </c>
@@ -1732,19 +1732,19 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_21;31;20.json</t>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_21;41;27.json</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached on whether to select pajama day or formal day for spirit week.
+MSG: A compromise was reached for spirit week.
 </t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t xml:space="preserve">no_consensus, </t>
+          <t xml:space="preserve">they_came_to_a_compromise, </t>
         </is>
       </c>
     </row>
@@ -1754,19 +1754,19 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;45;31.json</t>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;47;01.json</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: Pajama day was selected as the theme for spirit week.
+MSG: The theme for spirit week is "Pajama Meets Formal," which was a result of a compromise between the two sides.
 </t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t xml:space="preserve">pajama_day_was_selected, </t>
+          <t xml:space="preserve">they_came_to_a_compromise, </t>
         </is>
       </c>
     </row>
@@ -1776,19 +1776,19 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_20;48;07.json</t>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_20;51;12.json</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: Pajama day was selected for spirit week.
+MSG: There was no consensus reached on the theme for spirit week.
 </t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t xml:space="preserve">pajama_day_was_selected, </t>
+          <t xml:space="preserve">no_consensus, </t>
         </is>
       </c>
     </row>
@@ -1798,13 +1798,13 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;31;07.json</t>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;01;17.json</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached between Amy and Alice regarding the theme for spirit week.
+MSG: There was no consensus reached on the theme for spirit week.
 </t>
         </is>
       </c>
@@ -1820,13 +1820,13 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_20;43;12.json</t>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_21;51;12.json</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The theme for spirit week has been decided as pajama day.
+MSG: Pajama Day was selected as the theme for spirit week! Enjoy the fun with fancy accessories.
 </t>
         </is>
       </c>
@@ -1842,13 +1842,13 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;51;27.json</t>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_21;59;07.json</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: Pajama Day was selected for spirit week.
+MSG: Pajama day was selected for spirit week.
 </t>
         </is>
       </c>
@@ -1864,13 +1864,13 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;48;53.json</t>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;00;39.json</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: Pajama Day was selected as the theme for spirit week.
+MSG: Pajama day was selected as the theme for spirit week.
 </t>
         </is>
       </c>
@@ -1886,19 +1886,19 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_20;47;02.json</t>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;03;56.json</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached on the theme for spirit week.
+MSG: The decision was made through a compromise, incorporating elements from both Pajama Day and a formal celebration.
 </t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t xml:space="preserve">no_consensus, </t>
+          <t xml:space="preserve">they_came_to_a_compromise, </t>
         </is>
       </c>
     </row>
@@ -1908,13 +1908,13 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;34;09.json</t>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;31;07.json</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: Based on the information provided, there was no consensus reached on the theme for spirit week.
+MSG: There was no consensus reached on the theme for spirit week.
 </t>
         </is>
       </c>
@@ -1930,19 +1930,19 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_21;33;39.json</t>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;09;20.json</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached on the theme for spirit week.
+MSG: Pajama Day was selected for spirit week.
 </t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t xml:space="preserve">no_consensus, </t>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
         </is>
       </c>
     </row>
@@ -1952,13 +1952,13 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;30;33.json</t>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;13;45.json</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: Pajama Day was selected as the theme for spirit week.
+MSG: The theme for spirit week is Pajama Day.
 </t>
         </is>
       </c>
@@ -1974,7 +1974,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_20;46;24.json</t>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;01;46.json</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -1996,19 +1996,19 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;21;08.json</t>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_18;51;35.json</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: Pajama Day was selected as the theme for spirit week.
+MSG: There was no consensus reached between the groups regarding the spirit week theme.
 </t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t xml:space="preserve">pajama_day_was_selected, </t>
+          <t xml:space="preserve">no_consensus, </t>
         </is>
       </c>
     </row>
@@ -2018,13 +2018,13 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;21;57.json</t>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_18;51;03.json</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached on the theme for spirit week.
+MSG: There was no consensus reached between the two parties regarding the theme for spirit week.
 </t>
         </is>
       </c>
@@ -2040,19 +2040,19 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_18;49;40.json</t>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;54;08.json</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: Pajama Day was selected for spirit week.
+MSG: There was no consensus reached for the theme of spirit week.
 </t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t xml:space="preserve">pajama_day_was_selected, </t>
+          <t xml:space="preserve">no_consensus, </t>
         </is>
       </c>
     </row>
@@ -2062,19 +2062,19 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;44;03.json</t>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;08;34.json</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached on the theme for spirit week.
+MSG: Pajama Day was selected for spirit week.
 </t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t xml:space="preserve">no_consensus, </t>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
         </is>
       </c>
     </row>
@@ -2084,13 +2084,13 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_21;40;13.json</t>
+          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;32;52.json</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached on the theme for spirit week.
+MSG: There was no consensus reached between the participants on the theme for spirit week.
 </t>
         </is>
       </c>
@@ -2106,13 +2106,13 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;44;31.json</t>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;09;45.json</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached regarding the theme for spirit week.
+MSG: There was no consensus reached for the spirit week theme.
 </t>
         </is>
       </c>
@@ -2128,19 +2128,19 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_10_2025 at_21;35;02.json</t>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;16;19.json</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: There was no consensus reached on the theme for spirit week.
+MSG: The theme for spirit week has been decided: Pajama Day was selected.
 </t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t xml:space="preserve">no_consensus, </t>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
         </is>
       </c>
     </row>
@@ -2150,7 +2150,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;24;18.json</t>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_20;48;36.json</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2172,17 +2172,1557 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;55;11.json</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The discussion concluded without a consensus on whether to select formal day or pajama day for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_consensus, </t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_21;57;23.json</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: Since Alice and Amy did not reach an agreement, there was no consensus on selecting the theme for spirit week between formal day and pajama day.
+</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_consensus, </t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;50;29.json</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: Pajama day was selected for spirit week this Friday.
+</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;12;01.json</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: There was no consensus on the theme for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_consensus, </t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;15;50.json</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: Pajama Day was selected as the theme for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;11;30.json</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: There was no consensus reached regarding the theme for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_consensus, </t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;46;07.json</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: Pajama Day was selected for the spirit week's theme.
+</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;35;39.json</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: There was no consensus reached on the theme for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_consensus, </t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;43;31.json</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: There was no consensus reached regarding the theme for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_consensus, </t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;24;50.json</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: Pajama day was selected for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;20;24.json</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The theme for spirit week was decided upon as a compromise, combining both pajama day and formal day. This approach allows for creativity and inclusivity, catering to various student preferences and situations.
+</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t xml:space="preserve">they_came_to_a_compromise, </t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_20;47;38.json</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: There was no consensus reached on the theme for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_consensus, </t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;00;06.json</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The two have come to a compromise by merging Pajama Day with elements of Formal Day. The Spirit Week theme will reflect both ideas.
+</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t xml:space="preserve">they_came_to_a_compromise, </t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;29;56.json</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The decision for spirit week resulted in a compromise, incorporating both Pajama Day and Formal Day into the plans.
+</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t xml:space="preserve">they_came_to_a_compromise, </t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_21;58;44.json</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: Pajama Day was selected for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_20;49;52.json</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The decision for spirit week was to come to a compromise, selecting a "Smart Casual Day" theme.
+</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t xml:space="preserve">they_came_to_a_compromise, </t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_21;32;46.json</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The decision was to propose a plan that incorporates both pajama day and formal day, suggesting that they have come to a compromise for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t xml:space="preserve">they_came_to_a_compromise, </t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_21;36;22.json</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: Pajama day was selected as the theme for spirit week. Everyone can look forward to a fun and comfortable day dressed in their favorite pajamas!
+</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;22;37.json</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: There was no consensus on the theme for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_consensus, </t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_21;39;40.json</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The discussion did not result in a consensus on whether to select formal day or pajama day for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_consensus, </t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_21;56;03.json</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: Pajama Day was selected for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_21;34;23.json</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: No consensus was reached on the theme for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_consensus, </t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;28;30.json</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The decision for spirit week is a compromise that incorporates elements from both Pajama Day and Formal Day.
+</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t xml:space="preserve">they_came_to_a_compromise, </t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;03;27.json</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: Pajama day was selected as the theme for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="n">
+        <v>102</v>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;04;19.json</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: They came to a compromise for the theme of spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">they_came_to_a_compromise, </t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="n">
+        <v>103</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;49;33.json</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: There was no consensus reached on the theme for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_consensus, </t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_21;31;20.json</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: There was no consensus reached regarding the theme for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_consensus, </t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="n">
+        <v>105</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;45;31.json</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: Pajama day was selected for spirit week!
+</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="n">
+        <v>106</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_20;48;07.json</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: Pajama Day was selected for spirit week!
+</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="n">
+        <v>107</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;31;07.json</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: There was no consensus reached on the theme for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_consensus, </t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_20;43;12.json</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The theme for spirit week is pajama day.
+</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="n">
+        <v>109</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;03;04.json</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: There was no consensus reached on the theme for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_consensus, </t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_21;54;32.json</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The theme for spirit week has been decided as Pajama Day.
+</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="n">
+        <v>111</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;51;27.json</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: Pajama Day was selected for spirit week. Everyone can look forward to a cozy and fun Friday!
+</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="n">
+        <v>112</v>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;08;10.json</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: There was no consensus reached on the theme for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_consensus, </t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="n">
+        <v>113</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_21;59;34.json</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: There was no consensus reached on the theme for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_consensus, </t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="n">
+        <v>114</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;48;53.json</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: Pajama Day was selected for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="n">
+        <v>115</v>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_20;47;02.json</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: Both agreed that Pajama Day was selected for Friday during spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="n">
+        <v>116</v>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_21;54;05.json</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: Pajama Day was selected for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="n">
+        <v>117</v>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;34;09.json</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: There was no consensus reached on the theme for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_consensus, </t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="n">
+        <v>118</v>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;04;54.json</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The theme for spirit week was selected as "Dress Your PJs" day, which incorporates elements of both comfort and formality.
+</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="n">
+        <v>119</v>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_21;33;39.json</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: Pajama Day was selected as the theme for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;02;11.json</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: Since there was no agreement reached during the discussion, there is no consensus on the theme for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_consensus, </t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="n">
+        <v>121</v>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;18;53.json</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: There was no consensus reached on the theme for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_consensus, </t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="n">
+        <v>122</v>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;18;34.json</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: Pajama Day was selected for spirit week!
+</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="n">
+        <v>123</v>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;21;13.json</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: There was no consensus on the theme for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_consensus, </t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="n">
+        <v>124</v>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;30;33.json</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: Pajama Day was selected for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="n">
+        <v>125</v>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_21;52;13.json</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: They came to a compromise for the spirit week theme.
+</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t xml:space="preserve">they_came_to_a_compromise, </t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="n">
+        <v>126</v>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_20;46;24.json</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: There was no consensus on the theme for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_consensus, </t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="n">
+        <v>127</v>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;21;08.json</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: Pajama Day was selected as the theme for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;21;57.json</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: There was no consensus reached regarding the theme for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_consensus, </t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="n">
+        <v>129</v>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_21;50;24.json</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: There was no consensus on the theme for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_consensus, </t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="n">
+        <v>130</v>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_18;49;40.json</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: Pajama Day was selected as the theme for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="n">
+        <v>131</v>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;44;03.json</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: There was no consensus reached on the theme for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_consensus, </t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="n">
+        <v>132</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_21;40;13.json</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: There was no consensus reached on the theme for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_consensus, </t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="n">
+        <v>133</v>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;19;44.json</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: Pajama day was selected for the theme of spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_21;56;34.json</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: Pajama Day was selected for spirit week. Enjoy the cozy and fun atmosphere!
+</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="n">
+        <v>135</v>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_15;44;31.json</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: There was no consensus reached on the theme for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_consensus, </t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="n">
+        <v>136</v>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;08;56.json</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: There was no consensus on the theme for spirit week. Therefore, no theme was selected.
+</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_consensus, </t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="n">
+        <v>137</v>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;19;22.json</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The decision was to blend both ideas, allowing Pajama Day as the main theme with an option for kids to dress up formally. They came to a compromise.
+</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t xml:space="preserve">they_came_to_a_compromise, </t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="1" t="n">
+        <v>138</v>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_10_2025 at_21;35;02.json</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: There was no consensus reached on the theme for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_consensus, </t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="1" t="n">
+        <v>139</v>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_08_2025 at_20;24;18.json</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: There was no consensus reached for the theme of spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_consensus, </t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;14;10.json</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: Pajama day was selected for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="1" t="n">
+        <v>141</v>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_21;02;23.json</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: There was no consensus reached on the theme for spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_consensus, </t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="1" t="n">
+        <v>142</v>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;07;26.json</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: Pajama Day was selected as the theme for spirit week!
+</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pajama_day_was_selected, </t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="1" t="n">
+        <v>143</v>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;10;34.json</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: They came to a compromise by blending elements of both Pajama Day and Formal Day to create a unique and inclusive experience for the spirit week.
+</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t xml:space="preserve">they_came_to_a_compromise, </t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="1" t="n">
+        <v>144</v>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;13;16.json</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: There was no consensus reached in the discussion for the spirit week theme.
+</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_consensus, </t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
           <t>./Warehouse/BB/run4o_test_02_10_2025 at_21;38;50.json</t>
         </is>
       </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t xml:space="preserve">MSG: None
-MSG: They came to a compromise regarding the spirit week theme.
-</t>
-        </is>
-      </c>
-      <c r="D80" t="inlineStr">
+      <c r="C147" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: They came to a compromise for spirit week. Both Pajama Day and Formal Day will be part of the week's themes.
+</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t xml:space="preserve">they_came_to_a_compromise, </t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;11;01.json</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The theme for Spirit Week is a compromise that combines both Formal Day and Pajama Day elements.
+</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t xml:space="preserve">they_came_to_a_compromise, </t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="1" t="n">
+        <v>147</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;12;49.json</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The decision for spirit week is a compromise between pajama day and formal day, resulting in a pajama-themed formal day.
+</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t xml:space="preserve">they_came_to_a_compromise, </t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="1" t="n">
+        <v>148</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>./Warehouse/BB/run4o_test_02_21_2025 at_22;05;54.json</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The decision for spirit week was a compromise, blending elements from both themes to create a unique and engaging experience.
+</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
         <is>
           <t xml:space="preserve">they_came_to_a_compromise, </t>
         </is>

</xml_diff>